<commit_message>
Data Master Kota Di indonesia
Data Master Kota Di indonesia
</commit_message>
<xml_diff>
--- a/DATA MASTER KOTA DI INDONESIA.xlsx
+++ b/DATA MASTER KOTA DI INDONESIA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="32"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="JABAR" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="283">
   <si>
     <t>No</t>
   </si>
@@ -614,19 +614,316 @@
   </si>
   <si>
     <t>Kota Tangerang Selatan</t>
+  </si>
+  <si>
+    <t>kota</t>
+  </si>
+  <si>
+    <t>Kabupaten Bengkalis</t>
+  </si>
+  <si>
+    <t>Kabupaten Indragiri Hilir</t>
+  </si>
+  <si>
+    <t>Kabupaten Indragiri Hulu</t>
+  </si>
+  <si>
+    <t>Kabupaten Kampar</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepulauan Meranti</t>
+  </si>
+  <si>
+    <t>Kabupaten Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>Kabupaten Pelalawan</t>
+  </si>
+  <si>
+    <t>Kabupaten Rokan Hilir</t>
+  </si>
+  <si>
+    <t>Kabupaten Rokan Hulu</t>
+  </si>
+  <si>
+    <t>Kabupaten Siak</t>
+  </si>
+  <si>
+    <t>Kota Dumai</t>
+  </si>
+  <si>
+    <t>Kota Pekanbaru</t>
+  </si>
+  <si>
+    <t>Kabupaten Paser</t>
+  </si>
+  <si>
+    <t>Kabupaten Kutai Kartanegara</t>
+  </si>
+  <si>
+    <t>Kabupaten Berau</t>
+  </si>
+  <si>
+    <t>Kabupaten Kutai Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Kutai Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Penajam Paser Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Mahakam Ulu</t>
+  </si>
+  <si>
+    <t>Kota Balikpapan</t>
+  </si>
+  <si>
+    <t>Kota Samarinda</t>
+  </si>
+  <si>
+    <t>Kota Bontang</t>
+  </si>
+  <si>
+    <t>Kabupaten Asahan</t>
+  </si>
+  <si>
+    <t>Kabupaten Batubara</t>
+  </si>
+  <si>
+    <t>Kabupaten Dairi</t>
+  </si>
+  <si>
+    <t>Kabupaten Deli Serdang</t>
+  </si>
+  <si>
+    <t>Kabupaten Humbang Hasundutan</t>
+  </si>
+  <si>
+    <t>Kabupaten Karo</t>
+  </si>
+  <si>
+    <t>Kabupaten Labuhanbatu</t>
+  </si>
+  <si>
+    <t>Kabupaten Labuhanbatu Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Labuhanbatu Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Langkat</t>
+  </si>
+  <si>
+    <t>Kabupaten Mandailing Natal</t>
+  </si>
+  <si>
+    <t>Kabupaten Nias</t>
+  </si>
+  <si>
+    <t>Kabupaten Nias Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Nias Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Nias Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Padang Lawas</t>
+  </si>
+  <si>
+    <t>Kabupaten Padang Lawas Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Pakpak Bharat</t>
+  </si>
+  <si>
+    <t>Kabupaten Samosir</t>
+  </si>
+  <si>
+    <t>Kabupaten Serdang Bedagai</t>
+  </si>
+  <si>
+    <t>Kabupaten Simalungun</t>
+  </si>
+  <si>
+    <t>Kabupaten Tapanuli Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Tapanuli Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Tapanuli Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Toba Samosir</t>
+  </si>
+  <si>
+    <t>Kota Binjai</t>
+  </si>
+  <si>
+    <t>Kota Gunungsitoli</t>
+  </si>
+  <si>
+    <t>Kota Medan</t>
+  </si>
+  <si>
+    <t>Kota Padangsidempuan</t>
+  </si>
+  <si>
+    <t>Kota Pematang Siantar</t>
+  </si>
+  <si>
+    <t>Kota Sibolga</t>
+  </si>
+  <si>
+    <t>Kota Tanjung Balai</t>
+  </si>
+  <si>
+    <t>Kota Tebing Tinggi</t>
+  </si>
+  <si>
+    <t>Kabupaten Kupang</t>
+  </si>
+  <si>
+    <t>Kabupaten Timor Tengah Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Timor Tengah Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Belu</t>
+  </si>
+  <si>
+    <t>Kabupaten Alor</t>
+  </si>
+  <si>
+    <t>Kabupaten Flores Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Sikka</t>
+  </si>
+  <si>
+    <t>Kabupaten Ende</t>
+  </si>
+  <si>
+    <t>Kabupaten Ngada</t>
+  </si>
+  <si>
+    <t>Kabupaten Manggarai</t>
+  </si>
+  <si>
+    <t>Kabupaten Sumba Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Sumba Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Lembata</t>
+  </si>
+  <si>
+    <t>Kabupaten Rote Ndao</t>
+  </si>
+  <si>
+    <t>Kabupaten Manggarai Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Nagekeo</t>
+  </si>
+  <si>
+    <t>Kabupaten Sumba Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Sumba Barat Daya</t>
+  </si>
+  <si>
+    <t>Kabupaten Manggarai Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Sabu Raijua</t>
+  </si>
+  <si>
+    <t>Kabupaten Malaka</t>
+  </si>
+  <si>
+    <t>Kota Kupang</t>
+  </si>
+  <si>
+    <t>Kabupaten Maluku Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Maluku Tenggara</t>
+  </si>
+  <si>
+    <t>Kabupaten Maluku Tenggara Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Buru</t>
+  </si>
+  <si>
+    <t>Kabupaten Seram Bagian Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Seram Bagian Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepulauan Aru</t>
+  </si>
+  <si>
+    <t>Kabupaten Maluku Barat Daya</t>
+  </si>
+  <si>
+    <t>Kabupaten Buru Selatan</t>
+  </si>
+  <si>
+    <t>Kota Ambon</t>
+  </si>
+  <si>
+    <t>Kota Tual</t>
+  </si>
+  <si>
+    <t>Kabupaten Bintan</t>
+  </si>
+  <si>
+    <t>Kabupaten Karimun</t>
+  </si>
+  <si>
+    <t>Kabupaten Natuna</t>
+  </si>
+  <si>
+    <t>Kabupaten Lingga</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepulauan Anambas</t>
+  </si>
+  <si>
+    <t>Kota Batam</t>
+  </si>
+  <si>
+    <t>Kota Tanjungpinang</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -675,12 +972,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1293,72 +1593,1214 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="57">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="1">
+        <v>14.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="1">
+        <v>14.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="57">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="1">
+        <v>14.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="42.75">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" s="1">
+        <v>14.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="71.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="1">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="1">
+        <v>14.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="1">
+        <v>14.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="1">
+        <v>14.07</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="57">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="1">
+        <v>14.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.5">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" s="1">
+        <v>14.72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="42.75">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C13" s="1">
+        <v>14.71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.75">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>64.010000000000005</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>64.02</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42.75">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>64.03</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="42.75">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="42.75">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64.08</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="71.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>64.09</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>64.11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="42.75">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="42.75">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>64.72</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>64.739999999999995</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.75">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12.09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12.19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="42.75">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" s="1">
+        <v>12.07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="85.5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="1">
+        <v>12.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="1">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="71.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="1">
+        <v>12.22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="71.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="42.75">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="1">
+        <v>12.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="1">
+        <v>12.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.5">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="42.75">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="42.75">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12.14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="42.75">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" s="1">
+        <v>12.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="57">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" s="1">
+        <v>12.21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="71.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" s="1">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="57">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C19" s="1">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="42.75">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="1">
+        <v>12.17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="57">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="1">
+        <v>12.18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="57">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="57">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="1">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="57">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C24" s="1">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="57">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C25" s="1">
+        <v>12.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="42.75">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C26" s="1">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28.5">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="1">
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="42.75">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C28" s="1">
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.5">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C29" s="1">
+        <v>12.71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="57">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C30" s="1">
+        <v>12.77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="57">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C31" s="1">
+        <v>12.72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.5">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C32" s="1">
+        <v>12.73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="42.75">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C33" s="1">
+        <v>12.74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="42.75">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C34" s="1">
+        <v>12.76</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.75">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>53.01</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="71.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>53.02</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="71.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>53.03</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>53.04</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>53.05</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>53.06</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>53.07</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>53.08</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="42.75">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>53.09</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="57">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>53.1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>53.11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="57">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>53.12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="42.75">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>53.13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="42.75">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>53.14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="57">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>53.15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="42.75">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>53.16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="57">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>53.17</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="71.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>53.18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="57">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>53.19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="42.75">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>53.2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="42.75">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>53.21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.5">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>53.71</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="57">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>81.010000000000005</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="71.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>81.02</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="71.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>81.03</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>81.040000000000006</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="71.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>81.05</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="71.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>81.06</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>81.069999999999993</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="71.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>81.08</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="42.75">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>81.09</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>81.709999999999994</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.5">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>81.72</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.75">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>21.01</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="42.75">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>21.02</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42.75">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>21.03</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="42.75">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>21.04</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="85.5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>21.05</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>21.71</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="42.75">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>21.72</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1367,10 +2809,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2438,7 +3886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Database Update Kota Di Indonesia
Database Update Kota Di Indonesia
</commit_message>
<xml_diff>
--- a/DATA MASTER KOTA DI INDONESIA.xlsx
+++ b/DATA MASTER KOTA DI INDONESIA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="15" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="JABAR" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="320">
   <si>
     <t>No</t>
   </si>
@@ -905,6 +905,117 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Kabupaten Lombok Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Lombok Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Lombok Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Sumbawa</t>
+  </si>
+  <si>
+    <t>Kabupaten Dompu</t>
+  </si>
+  <si>
+    <t>Kabupaten Bima</t>
+  </si>
+  <si>
+    <t>Kabupaten Sumbawa Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Lombok Utara</t>
+  </si>
+  <si>
+    <t>Kota Mataram</t>
+  </si>
+  <si>
+    <t>Kota Bima</t>
+  </si>
+  <si>
+    <t>Kabupaten Sambas</t>
+  </si>
+  <si>
+    <t>Kabupaten Mempawah</t>
+  </si>
+  <si>
+    <t>Kabupaten Sanggau</t>
+  </si>
+  <si>
+    <t>Kabupaten Ketapang</t>
+  </si>
+  <si>
+    <t>Kabupaten Sintang</t>
+  </si>
+  <si>
+    <t>Kabupaten Kapuas Hulu</t>
+  </si>
+  <si>
+    <t>Kabupaten Bengkayang</t>
+  </si>
+  <si>
+    <t>Kabupaten Landak</t>
+  </si>
+  <si>
+    <t>Kabupaten Sekadau</t>
+  </si>
+  <si>
+    <t>Kabupaten Melawi</t>
+  </si>
+  <si>
+    <t>Kabupaten Kayong Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Kubu Raya</t>
+  </si>
+  <si>
+    <t>Kota Pontianak</t>
+  </si>
+  <si>
+    <t>Kota Singkawang</t>
+  </si>
+  <si>
+    <t>Kabupaten Tanah Laut</t>
+  </si>
+  <si>
+    <t>Kabupaten Kotabaru</t>
+  </si>
+  <si>
+    <t>Kabupaten Banjar</t>
+  </si>
+  <si>
+    <t>Kabupaten Barito Kuala</t>
+  </si>
+  <si>
+    <t>Kabupaten Tapin</t>
+  </si>
+  <si>
+    <t>Kabupaten Hulu Sungai Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Hulu Sungai Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Hulu Sungai Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Tabalong</t>
+  </si>
+  <si>
+    <t>Kabupaten Tanah Bumbu</t>
+  </si>
+  <si>
+    <t>Kabupaten Balangan</t>
+  </si>
+  <si>
+    <t>Kota Banjarmasin</t>
+  </si>
+  <si>
+    <t>Kota Banjarbaru</t>
   </si>
 </sst>
 </file>
@@ -2809,7 +2920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -2849,12 +2960,185 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.75">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>61.01</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>61.02</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="57">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>61.03</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>61.04</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="42.75">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>61.05</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>61.06</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>61.07</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="42.75">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>61.08</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="42.75">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>61.09</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="42.75">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>61.1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>61.11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="42.75">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>61.12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="42.75">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>61.71</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="42.75">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>61.72</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3277,24 +3561,305 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="57">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>52.01</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>52.02</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="57">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>52.03</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>52.04</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="42.75">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>52.05</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>52.06</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="71.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>52.07</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>52.08</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.5">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>52.71</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>52.72</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="57">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>63.01</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>63.02</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42.75">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>63.03</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>63.04</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>63.05</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="57">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>63.06</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="57">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>63.07</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>63.08</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="57">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>63.09</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="57">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>63.1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>63.11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="42.75">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>63.71</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="42.75">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>63.72</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3315,7 +3880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
add new master data
</commit_message>
<xml_diff>
--- a/DATA MASTER KOTA DI INDONESIA.xlsx
+++ b/DATA MASTER KOTA DI INDONESIA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dian Insani\Documents\SEMESTER 3\Proyek\KOTA INDONESIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hibatullah\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="15" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7800" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="JABAR" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="299">
   <si>
     <t>No</t>
   </si>
@@ -904,125 +904,62 @@
     <t>Kota Tanjungpinang</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Kabupaten Lombok Barat</t>
-  </si>
-  <si>
-    <t>Kabupaten Lombok Tengah</t>
-  </si>
-  <si>
-    <t>Kabupaten Lombok Timur</t>
-  </si>
-  <si>
-    <t>Kabupaten Sumbawa</t>
-  </si>
-  <si>
-    <t>Kabupaten Dompu</t>
-  </si>
-  <si>
-    <t>Kabupaten Bima</t>
-  </si>
-  <si>
-    <t>Kabupaten Sumbawa Barat</t>
-  </si>
-  <si>
-    <t>Kabupaten Lombok Utara</t>
-  </si>
-  <si>
-    <t>Kota Mataram</t>
-  </si>
-  <si>
-    <t>Kota Bima</t>
-  </si>
-  <si>
-    <t>Kabupaten Sambas</t>
-  </si>
-  <si>
-    <t>Kabupaten Mempawah</t>
-  </si>
-  <si>
-    <t>Kabupaten Sanggau</t>
-  </si>
-  <si>
-    <t>Kabupaten Ketapang</t>
-  </si>
-  <si>
-    <t>Kabupaten Sintang</t>
-  </si>
-  <si>
-    <t>Kabupaten Kapuas Hulu</t>
-  </si>
-  <si>
-    <t>Kabupaten Bengkayang</t>
-  </si>
-  <si>
-    <t>Kabupaten Landak</t>
-  </si>
-  <si>
-    <t>Kabupaten Sekadau</t>
-  </si>
-  <si>
-    <t>Kabupaten Melawi</t>
-  </si>
-  <si>
-    <t>Kabupaten Kayong Utara</t>
-  </si>
-  <si>
-    <t>Kabupaten Kubu Raya</t>
-  </si>
-  <si>
-    <t>Kota Pontianak</t>
-  </si>
-  <si>
-    <t>Kota Singkawang</t>
-  </si>
-  <si>
-    <t>Kabupaten Tanah Laut</t>
-  </si>
-  <si>
-    <t>Kabupaten Kotabaru</t>
-  </si>
-  <si>
-    <t>Kabupaten Banjar</t>
-  </si>
-  <si>
-    <t>Kabupaten Barito Kuala</t>
-  </si>
-  <si>
-    <t>Kabupaten Tapin</t>
-  </si>
-  <si>
-    <t>Kabupaten Hulu Sungai Selatan</t>
-  </si>
-  <si>
-    <t>Kabupaten Hulu Sungai Tengah</t>
-  </si>
-  <si>
-    <t>Kabupaten Hulu Sungai Utara</t>
-  </si>
-  <si>
-    <t>Kabupaten Tabalong</t>
-  </si>
-  <si>
-    <t>Kabupaten Tanah Bumbu</t>
-  </si>
-  <si>
-    <t>Kabupaten Balangan</t>
-  </si>
-  <si>
-    <t>Kota Banjarmasin</t>
-  </si>
-  <si>
-    <t>Kota Banjarbaru</t>
+    <t>Kabupaten Banyuasin</t>
+  </si>
+  <si>
+    <t>Kabupaten Empat Lawang</t>
+  </si>
+  <si>
+    <t>Kabupaten Lahat</t>
+  </si>
+  <si>
+    <t>Kabupaten Muara Enim</t>
+  </si>
+  <si>
+    <t>Kabupaten Musi Banyuasin</t>
+  </si>
+  <si>
+    <t>Kabupaten Musi Rawas</t>
+  </si>
+  <si>
+    <t>Kabupaten Musi Rawas Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Ogan Ilir</t>
+  </si>
+  <si>
+    <t>Kabupaten Ogan Komering Ilir</t>
+  </si>
+  <si>
+    <t>Kabupaten Ogan Komering Ulu</t>
+  </si>
+  <si>
+    <t>Kabupaten Ogan Komering Ulu Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Ogan Komering Ulu Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Penukal Arab Lematang Ilir</t>
+  </si>
+  <si>
+    <t>Kota Lubuk Linggau</t>
+  </si>
+  <si>
+    <t>Kota Pagar Alam</t>
+  </si>
+  <si>
+    <t>Kota Palembang</t>
+  </si>
+  <si>
+    <t>Kota Prabumulih</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1035,6 +972,11 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1083,7 +1025,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1092,6 +1034,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1399,7 +1347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42.75">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1410,7 +1358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1421,7 +1369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42.75">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1432,7 +1380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1443,7 +1391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.5">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1454,7 +1402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1465,7 +1413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="42.75">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1476,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="57">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1487,7 +1435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="42.75">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1498,7 +1446,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="57">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1509,7 +1457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="57">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1520,7 +1468,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1531,7 +1479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="42.75">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1542,7 +1490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1553,7 +1501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1564,7 +1512,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="42.75">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1575,7 +1523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="57">
+    <row r="18" spans="1:3" ht="28.5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1586,7 +1534,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="57">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1597,7 +1545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.5">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1608,7 +1556,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="42.75">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1619,7 +1567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="42.75">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1630,7 +1578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.5">
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1641,7 +1589,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.5">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1652,7 +1600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.5">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1663,7 +1611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.5">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1674,7 +1622,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="42.75">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1685,7 +1633,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.5">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2022,7 +1970,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42.75">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2033,7 +1981,7 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2044,7 +1992,7 @@
         <v>12.19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.5">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2055,7 +2003,7 @@
         <v>12.11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="42.75">
+    <row r="5" spans="1:3" ht="28.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2066,7 +2014,7 @@
         <v>12.07</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="85.5">
+    <row r="6" spans="1:3" ht="28.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2077,7 +2025,7 @@
         <v>12.16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.5">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2088,7 +2036,7 @@
         <v>12.06</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="57">
+    <row r="8" spans="1:3" ht="28.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2099,7 +2047,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="71.25">
+    <row r="9" spans="1:3" ht="28.5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2110,7 +2058,7 @@
         <v>12.22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="71.25">
+    <row r="10" spans="1:3" ht="28.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2121,7 +2069,7 @@
         <v>12.23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="42.75">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2132,7 +2080,7 @@
         <v>12.05</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="57">
+    <row r="12" spans="1:3" ht="28.5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2143,7 +2091,7 @@
         <v>12.13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.5">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2154,7 +2102,7 @@
         <v>12.04</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="42.75">
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2165,7 +2113,7 @@
         <v>12.25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="42.75">
+    <row r="15" spans="1:3" ht="28.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2176,7 +2124,7 @@
         <v>12.14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="42.75">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2187,7 +2135,7 @@
         <v>12.24</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="57">
+    <row r="17" spans="1:3" ht="28.5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2198,7 +2146,7 @@
         <v>12.21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="71.25">
+    <row r="18" spans="1:3" ht="28.5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2209,7 +2157,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="57">
+    <row r="19" spans="1:3" ht="28.5">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2220,7 +2168,7 @@
         <v>12.15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42.75">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2231,7 +2179,7 @@
         <v>12.17</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="57">
+    <row r="21" spans="1:3" ht="28.5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2242,7 +2190,7 @@
         <v>12.18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="57">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2253,7 +2201,7 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="57">
+    <row r="23" spans="1:3" ht="28.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2264,7 +2212,7 @@
         <v>12.03</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="57">
+    <row r="24" spans="1:3" ht="28.5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2275,7 +2223,7 @@
         <v>12.01</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="57">
+    <row r="25" spans="1:3" ht="28.5">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2286,7 +2234,7 @@
         <v>12.02</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="42.75">
+    <row r="26" spans="1:3" ht="28.5">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2297,7 +2245,7 @@
         <v>12.12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.5">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2308,7 +2256,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="42.75">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2319,7 +2267,7 @@
         <v>12.78</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.5">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2330,7 +2278,7 @@
         <v>12.71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="57">
+    <row r="30" spans="1:3" ht="28.5">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2341,7 +2289,7 @@
         <v>12.77</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="57">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2352,7 +2300,7 @@
         <v>12.72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="28.5">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2363,7 +2311,7 @@
         <v>12.73</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="42.75">
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2374,7 +2322,7 @@
         <v>12.74</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="42.75">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2831,7 +2779,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42.75">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2842,7 +2790,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="42.75">
+    <row r="3" spans="1:3" ht="28.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2853,7 +2801,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42.75">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2864,7 +2812,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="42.75">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2875,7 +2823,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="85.5">
+    <row r="6" spans="1:3" ht="42.75">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2886,7 +2834,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.5">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2897,7 +2845,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="42.75">
+    <row r="8" spans="1:3" ht="28.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2918,19 +2866,218 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.5">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>282</v>
+      </c>
+      <c r="C2" s="4">
+        <v>16.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="4">
+        <v>16.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="4">
+        <v>16.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="4">
+        <v>16.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="42.75">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="4">
+        <v>16.059999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C7" s="4">
+        <v>16.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="4">
+        <v>16.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" s="4">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.5">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C10" s="4">
+        <v>16.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="4">
+        <v>16.010000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="42.75">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C12" s="4">
+        <v>16.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="42.75">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C13" s="4">
+        <v>16.079999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.5">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C14" s="4">
+        <v>16.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="4">
+        <v>16.73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" s="4">
+        <v>16.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" s="4">
+        <v>16.71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C18" s="4">
+        <v>16.739999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2960,185 +3107,12 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="42.75">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>61.01</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="57">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>61.02</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="57">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>61.03</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="57">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>61.04</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="42.75">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>61.05</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="57">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>61.06</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="57">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>61.07</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="42.75">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>61.08</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="42.75">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>61.09</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="42.75">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>61.1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="57">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>61.11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="42.75">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>61.12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="42.75">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>61.71</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="42.75">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>61.72</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3169,7 +3143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42.75">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3180,7 +3154,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57">
+    <row r="3" spans="1:3" ht="28.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3191,7 +3165,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57">
+    <row r="4" spans="1:3" ht="28.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3202,7 +3176,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57">
+    <row r="5" spans="1:3" ht="28.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3213,7 +3187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="57">
+    <row r="6" spans="1:3" ht="28.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3224,7 +3198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57">
+    <row r="7" spans="1:3" ht="28.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3235,7 +3209,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="57">
+    <row r="8" spans="1:3" ht="28.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3246,7 +3220,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="57">
+    <row r="9" spans="1:3" ht="28.5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3257,7 +3231,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="42.75">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3268,7 +3242,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="42.75">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3279,7 +3253,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="57">
+    <row r="12" spans="1:3" ht="28.5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3290,7 +3264,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3301,7 +3275,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="57">
+    <row r="14" spans="1:3" ht="28.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3312,7 +3286,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="42.75">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3323,7 +3297,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57">
+    <row r="16" spans="1:3" ht="28.5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3334,7 +3308,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.5">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3345,7 +3319,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="57">
+    <row r="18" spans="1:3" ht="28.5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3356,7 +3330,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.5">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3367,7 +3341,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42.75">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3378,7 +3352,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="42.75">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3389,7 +3363,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="42.75">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3400,7 +3374,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="57">
+    <row r="23" spans="1:3" ht="28.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3411,7 +3385,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="57">
+    <row r="24" spans="1:3" ht="28.5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3422,7 +3396,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="42.75">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3433,7 +3407,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="42.75">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3444,7 +3418,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="57">
+    <row r="27" spans="1:3" ht="28.5">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3455,7 +3429,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="57">
+    <row r="28" spans="1:3" ht="28.5">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3466,7 +3440,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.5">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3477,7 +3451,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="42.75">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3488,7 +3462,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="42.75">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3499,7 +3473,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="42.75">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3510,7 +3484,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="28.5">
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3521,7 +3495,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="42.75">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3532,7 +3506,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="42.75">
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3543,7 +3517,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="28.5">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3561,305 +3535,24 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="57">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>52.01</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="57">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>52.02</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="57">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>52.03</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="57">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>52.04</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="42.75">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>52.05</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.5">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>52.06</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="71.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>52.07</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="57">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>52.08</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.5">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>52.71</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.5">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>52.72</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="57">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>63.01</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="57">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>63.02</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="42.75">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>63.03</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="57">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>63.04</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.5">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>63.05</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="57">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>63.06</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="57">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>63.07</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="57">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>63.08</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="57">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>63.09</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="57">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>63.1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="57">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>63.11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="42.75">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>63.71</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="42.75">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>63.72</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3880,7 +3573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
@@ -3986,7 +3679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42.75">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3997,7 +3690,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4008,7 +3701,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57">
+    <row r="4" spans="1:3" ht="28.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4019,7 +3712,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57">
+    <row r="5" spans="1:3" ht="28.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4030,7 +3723,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.5">
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4041,7 +3734,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.5">
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4052,7 +3745,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="42.75">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4063,7 +3756,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="57">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4074,7 +3767,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="42.75">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4085,7 +3778,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="57">
+    <row r="11" spans="1:3" ht="28.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4096,7 +3789,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="57">
+    <row r="12" spans="1:3" ht="28.5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4107,7 +3800,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="57">
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4118,7 +3811,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="57">
+    <row r="14" spans="1:3" ht="28.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4129,7 +3822,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57">
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4140,7 +3833,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="42.75">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4151,7 +3844,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="57">
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4162,7 +3855,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="57">
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4173,7 +3866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="42.75">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4184,7 +3877,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42.75">
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -4195,7 +3888,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="42.75">
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -4206,7 +3899,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="42.75">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4217,7 +3910,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="57">
+    <row r="23" spans="1:3" ht="28.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -4228,7 +3921,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="42.75">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -4239,7 +3932,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="57">
+    <row r="25" spans="1:3" ht="28.5">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -4250,7 +3943,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="42.75">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -4261,7 +3954,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="57">
+    <row r="27" spans="1:3" ht="28.5">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -4272,7 +3965,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="57">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -4283,7 +3976,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="57">
+    <row r="29" spans="1:3" ht="28.5">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -4294,7 +3987,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="57">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -4305,7 +3998,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.5">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -4316,7 +4009,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="28.5">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4327,7 +4020,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="28.5">
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -4338,7 +4031,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="42.75">
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4349,7 +4042,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="42.75">
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -4360,7 +4053,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="42.75">
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4371,7 +4064,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="28.5">
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -4382,7 +4075,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="42.75">
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4393,7 +4086,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="28.5">
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4705,7 +4398,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42.75">
+    <row r="2" spans="1:3" ht="28.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4716,7 +4409,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57">
+    <row r="3" spans="1:3" ht="28.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4727,7 +4420,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="42.75">
+    <row r="4" spans="1:3" ht="28.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4738,7 +4431,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="42.75">
+    <row r="5" spans="1:3" ht="28.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4749,7 +4442,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="42.75">
+    <row r="6" spans="1:3" ht="28.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4760,7 +4453,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="42.75">
+    <row r="7" spans="1:3" ht="28.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4771,7 +4464,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.5">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4812,7 +4505,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42.75">
+    <row r="2" spans="1:3" ht="28.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4823,7 +4516,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57">
+    <row r="3" spans="1:3" ht="28.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4834,7 +4527,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57">
+    <row r="4" spans="1:3" ht="28.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4845,7 +4538,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="42.75">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4856,7 +4549,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="71.25">
+    <row r="6" spans="1:3" ht="28.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4867,7 +4560,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="42.75">
+    <row r="7" spans="1:3" ht="28.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4878,7 +4571,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="57">
+    <row r="8" spans="1:3" ht="28.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4889,7 +4582,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="42.75">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4900,7 +4593,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="42.75">
+    <row r="10" spans="1:3" ht="28.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4911,7 +4604,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="42.75">
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4922,7 +4615,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="42.75">
+    <row r="12" spans="1:3" ht="28.5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4933,7 +4626,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="71.25">
+    <row r="13" spans="1:3" ht="42.75">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4944,7 +4637,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="57">
+    <row r="14" spans="1:3" ht="28.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4955,7 +4648,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="42.75">
+    <row r="15" spans="1:3" ht="28.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4966,7 +4659,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57">
+    <row r="16" spans="1:3" ht="28.5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4977,7 +4670,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="57">
+    <row r="17" spans="1:3" ht="28.5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4988,7 +4681,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="42.75">
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4999,7 +4692,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="42.75">
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -5010,7 +4703,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42.75">
+    <row r="20" spans="1:3" ht="28.5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5021,7 +4714,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="71.25">
+    <row r="21" spans="1:3" ht="42.75">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5032,7 +4725,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="71.25">
+    <row r="22" spans="1:3" ht="42.75">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5043,7 +4736,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="42.75">
+    <row r="23" spans="1:3" ht="28.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5054,7 +4747,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="57">
+    <row r="24" spans="1:3" ht="28.5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5065,7 +4758,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="42.75">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5076,7 +4769,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="42.75">
+    <row r="26" spans="1:3" ht="28.5">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5087,7 +4780,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="42.75">
+    <row r="27" spans="1:3" ht="28.5">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5098,7 +4791,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="42.75">
+    <row r="28" spans="1:3" ht="28.5">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5109,7 +4802,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="42.75">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5120,7 +4813,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="42.75">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5162,7 +4855,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="71.25">
+    <row r="2" spans="1:3" ht="28.5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5173,7 +4866,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="71.25">
+    <row r="3" spans="1:3" ht="28.5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5184,7 +4877,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57">
+    <row r="4" spans="1:3" ht="28.5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5195,7 +4888,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57">
+    <row r="5" spans="1:3" ht="28.5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5206,7 +4899,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="57">
+    <row r="6" spans="1:3" ht="28.5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -5217,7 +4910,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57">
+    <row r="7" spans="1:3" ht="28.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -5228,7 +4921,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="57">
+    <row r="8" spans="1:3" ht="28.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -5239,7 +4932,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="42.75">
+    <row r="9" spans="1:3" ht="28.5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -5250,7 +4943,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="57">
+    <row r="10" spans="1:3" ht="28.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -5261,7 +4954,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="57">
+    <row r="11" spans="1:3" ht="28.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5272,7 +4965,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="42.75">
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5283,7 +4976,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="71.25">
+    <row r="13" spans="1:3" ht="28.5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5294,7 +4987,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="57">
+    <row r="14" spans="1:3" ht="28.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5305,7 +4998,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="57">
+    <row r="15" spans="1:3" ht="28.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5316,7 +5009,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.5">
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
data master untuk kota di indonesia sudah lengkap
</commit_message>
<xml_diff>
--- a/DATA MASTER KOTA DI INDONESIA.xlsx
+++ b/DATA MASTER KOTA DI INDONESIA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7800" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7800" firstSheet="27" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="JABAR" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="487">
   <si>
     <t>No</t>
   </si>
@@ -953,13 +953,577 @@
   </si>
   <si>
     <t>Kota Prabumulih</t>
+  </si>
+  <si>
+    <t>Kabupaten Majene</t>
+  </si>
+  <si>
+    <t>Kabupaten Mamasa</t>
+  </si>
+  <si>
+    <t>Kabupaten Mamuju</t>
+  </si>
+  <si>
+    <t>Kabupaten Mamuju Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Mamuju Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Polewali Mandar</t>
+  </si>
+  <si>
+    <t>Kabupaten Bantaeng</t>
+  </si>
+  <si>
+    <t>Kabupaten Barru</t>
+  </si>
+  <si>
+    <t>Kabupaten Bone</t>
+  </si>
+  <si>
+    <t>Kabupaten Bulukumba</t>
+  </si>
+  <si>
+    <t>Kabupaten Enrekang</t>
+  </si>
+  <si>
+    <t>Kabupaten Gowa</t>
+  </si>
+  <si>
+    <t>Kabupaten Jeneponto</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepulauan Selayar</t>
+  </si>
+  <si>
+    <t>Kabupaten Luwu</t>
+  </si>
+  <si>
+    <t>Kabupaten Luwu Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Luwu Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Maros</t>
+  </si>
+  <si>
+    <t>Kabupaten Pangkajene dan Kepulauan</t>
+  </si>
+  <si>
+    <t>Kabupaten Pinrang</t>
+  </si>
+  <si>
+    <t>Kabupaten Sidenreng Rappang</t>
+  </si>
+  <si>
+    <t>Kabupaten Sinjai</t>
+  </si>
+  <si>
+    <t>Kabupaten Soppeng</t>
+  </si>
+  <si>
+    <t>Kabupaten Takalar</t>
+  </si>
+  <si>
+    <t>Kabupaten Tana Toraja</t>
+  </si>
+  <si>
+    <t>Kabupaten Toraja Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Wajo</t>
+  </si>
+  <si>
+    <t>Kota Makassar</t>
+  </si>
+  <si>
+    <t>Kota Palopo</t>
+  </si>
+  <si>
+    <t>Kota Parepare</t>
+  </si>
+  <si>
+    <t>Kode Wilayah</t>
+  </si>
+  <si>
+    <t>Kabupaten/Kota</t>
+  </si>
+  <si>
+    <t>Kabupaten Sambas</t>
+  </si>
+  <si>
+    <t>Kabupaten Mempawah</t>
+  </si>
+  <si>
+    <t>Kabupaten Sanggau</t>
+  </si>
+  <si>
+    <t>Kabupaten Ketapang</t>
+  </si>
+  <si>
+    <t>Kabupaten Sintang</t>
+  </si>
+  <si>
+    <t>Kabupaten Kapuas Hulu</t>
+  </si>
+  <si>
+    <t>Kabupaten Bengkayang</t>
+  </si>
+  <si>
+    <t>Kabupaten Landak</t>
+  </si>
+  <si>
+    <t>Kabupaten Sekadau</t>
+  </si>
+  <si>
+    <t>Kabupaten Melawi</t>
+  </si>
+  <si>
+    <t>Kabupaten Kayong Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Kubu Raya</t>
+  </si>
+  <si>
+    <t>Kota Pontianak</t>
+  </si>
+  <si>
+    <t>Kota Singkawang</t>
+  </si>
+  <si>
+    <t>Kabupaten Lombok Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Lombok Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Lombok Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Sumbawa</t>
+  </si>
+  <si>
+    <t>Kabupaten Dompu</t>
+  </si>
+  <si>
+    <t>Kabupaten Bima</t>
+  </si>
+  <si>
+    <t>Kabupaten Sumbawa Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Lombok Utara</t>
+  </si>
+  <si>
+    <t>Kota Mataram</t>
+  </si>
+  <si>
+    <t>Kota Bima</t>
+  </si>
+  <si>
+    <t>Kabupaten Tanah Laut</t>
+  </si>
+  <si>
+    <t>Kabupaten Kotabaru</t>
+  </si>
+  <si>
+    <t>Kabupaten Banjar</t>
+  </si>
+  <si>
+    <t>Kabupaten Barito Kuala</t>
+  </si>
+  <si>
+    <t>Kabupaten Tapin</t>
+  </si>
+  <si>
+    <t>Kabupaten Hulu Sungai Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Hulu Sungai Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Hulu Sungai Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Tabalong</t>
+  </si>
+  <si>
+    <t>Kabupaten Tanah Bumbu</t>
+  </si>
+  <si>
+    <t>Kabupaten Balangan</t>
+  </si>
+  <si>
+    <t>Kota Banjarmasin</t>
+  </si>
+  <si>
+    <t>Kota Banjarbaru</t>
+  </si>
+  <si>
+    <t>Kabupaten Kerinci</t>
+  </si>
+  <si>
+    <t>Kabupaten Merangin</t>
+  </si>
+  <si>
+    <t>Kabupaten Sarolangun</t>
+  </si>
+  <si>
+    <t>Kabupaten Batanghari</t>
+  </si>
+  <si>
+    <t>Kabupaten Muaro Jambi</t>
+  </si>
+  <si>
+    <t>Kabupaten Tanjung Jabung Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Tanjung Jabung Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Bungo</t>
+  </si>
+  <si>
+    <t>Kabupaten Tebo</t>
+  </si>
+  <si>
+    <t>Kota Jambi</t>
+  </si>
+  <si>
+    <t>Kota Sungai Penuh</t>
+  </si>
+  <si>
+    <t>Kabupaten Bolaang Mongondow</t>
+  </si>
+  <si>
+    <t>Kabupaten Bolaang Mondondow Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Bolaang Mondondow Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Bolaang Mondondow Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepulauan Sangihe</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepulauan Siau Tagulandang Biaro</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepulauan Talaud</t>
+  </si>
+  <si>
+    <t>Kabupaten Minahasa</t>
+  </si>
+  <si>
+    <t>Kabupaten Minahasa Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Minahasa Tenggara</t>
+  </si>
+  <si>
+    <t>Kabupaten Minahasa Utara</t>
+  </si>
+  <si>
+    <t>Kota Bitung</t>
+  </si>
+  <si>
+    <t>Kota Kotamobagu</t>
+  </si>
+  <si>
+    <t>Kota Manado</t>
+  </si>
+  <si>
+    <t>Kota Tomohon</t>
+  </si>
+  <si>
+    <t>Kabupaten Kotawaringin Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Kotawaringin Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Kapuas</t>
+  </si>
+  <si>
+    <t>Kabupaten Barito Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Barito Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Katingan</t>
+  </si>
+  <si>
+    <t>Kabupaten Seruyan</t>
+  </si>
+  <si>
+    <t>Kabupaten Sukamara</t>
+  </si>
+  <si>
+    <t>Kabupaten Lamandau</t>
+  </si>
+  <si>
+    <t>Kabupaten Gunung Mas</t>
+  </si>
+  <si>
+    <t>Kabupaten Pulang Pisau</t>
+  </si>
+  <si>
+    <t>Kabupaten Murung Raya</t>
+  </si>
+  <si>
+    <t>Kabupaten Barito Timur</t>
+  </si>
+  <si>
+    <t>Kota Palangka Raya</t>
+  </si>
+  <si>
+    <t>Kabupaten Bengkulu Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Rejang Lebong</t>
+  </si>
+  <si>
+    <t>Kabupaten Bengkulu Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Kaur</t>
+  </si>
+  <si>
+    <t>Kabupaten Seluma</t>
+  </si>
+  <si>
+    <t>Kabupaten Mukomuko</t>
+  </si>
+  <si>
+    <t>Kabupaten Lebong</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepahiang</t>
+  </si>
+  <si>
+    <t>Kabupaten Bangka</t>
+  </si>
+  <si>
+    <t>Kabupaten Belitung</t>
+  </si>
+  <si>
+    <t>Kabupaten Bangka Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Bangka Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Bangka Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Belitung Timur</t>
+  </si>
+  <si>
+    <t>Kota Pangkalpinang</t>
+  </si>
+  <si>
+    <t>Kabupaten Fakfak</t>
+  </si>
+  <si>
+    <t>Kabupaten Kaimana</t>
+  </si>
+  <si>
+    <t>Kabupaten Manokwari</t>
+  </si>
+  <si>
+    <t>Kabupaten Manokwari Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Maybrat</t>
+  </si>
+  <si>
+    <t>Kabupaten Pegunungan Arfak</t>
+  </si>
+  <si>
+    <t>Kabupaten Raja Ampat</t>
+  </si>
+  <si>
+    <t>Kabupaten Sorong</t>
+  </si>
+  <si>
+    <t>Kabupaten Sorong Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Tambrauw</t>
+  </si>
+  <si>
+    <t>Kabupaten Teluk Bintuni</t>
+  </si>
+  <si>
+    <t>Kabupaten Teluk Wondama</t>
+  </si>
+  <si>
+    <t>Kota Sorong</t>
+  </si>
+  <si>
+    <t>Kabupaten Bombana</t>
+  </si>
+  <si>
+    <t>Kabupaten Buton</t>
+  </si>
+  <si>
+    <t>Kabupaten Buton Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Buton Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Buton Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Kolaka</t>
+  </si>
+  <si>
+    <t>Kabupaten Kolaka Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Kolaka Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Konawe</t>
+  </si>
+  <si>
+    <t>Kabupaten Konawe Kepulauan</t>
+  </si>
+  <si>
+    <t>Kabupaten Konawe Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Konawe Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Muna</t>
+  </si>
+  <si>
+    <t>Kabupaten Muna Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Wakatobi</t>
+  </si>
+  <si>
+    <t>Kota Bau Bau</t>
+  </si>
+  <si>
+    <t>Kota Kendari</t>
+  </si>
+  <si>
+    <t>Kabupaten Banggai</t>
+  </si>
+  <si>
+    <t>Kabupaten Banggai Kepulauan</t>
+  </si>
+  <si>
+    <t>Kabupaten Banggai Laut</t>
+  </si>
+  <si>
+    <t>Kabupaten Buol</t>
+  </si>
+  <si>
+    <t>Kabupaten Donggala</t>
+  </si>
+  <si>
+    <t>Kabupaten Morowali</t>
+  </si>
+  <si>
+    <t>Kabupaten Morowali Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Parigi Moutong</t>
+  </si>
+  <si>
+    <t>Kabupaten Poso</t>
+  </si>
+  <si>
+    <t>Kabupaten Tojo Una-Una</t>
+  </si>
+  <si>
+    <t>Kabupaten Tolitoli</t>
+  </si>
+  <si>
+    <t>Kabupaten Sigi</t>
+  </si>
+  <si>
+    <t>Kota Palu</t>
+  </si>
+  <si>
+    <t>Kabupaten Gorontalo</t>
+  </si>
+  <si>
+    <t>Kabupaten Boalemo</t>
+  </si>
+  <si>
+    <t>Kabupaten Bone Bolango</t>
+  </si>
+  <si>
+    <t>Kabupaten Pohuwato</t>
+  </si>
+  <si>
+    <t>Kabupaten Gorontalo Utara</t>
+  </si>
+  <si>
+    <t>Kota Gorontalo</t>
+  </si>
+  <si>
+    <t>Kabupaten Halmahera Barat</t>
+  </si>
+  <si>
+    <t>Kabupaten Halmahera Tengah</t>
+  </si>
+  <si>
+    <t>Kabupaten Halmahera Utara</t>
+  </si>
+  <si>
+    <t>Kabupaten Halmahera Selatan</t>
+  </si>
+  <si>
+    <t>Kabupaten Kepulauan Sula</t>
+  </si>
+  <si>
+    <t>Kabupaten Halmahera Timur</t>
+  </si>
+  <si>
+    <t>Kabupaten Pulau Morotai</t>
+  </si>
+  <si>
+    <t>Kabupaten Pulau Taliabu</t>
+  </si>
+  <si>
+    <t>Kota Ternate</t>
+  </si>
+  <si>
+    <t>Kota Tidore Kepulauan</t>
+  </si>
+  <si>
+    <t>Kabupaten Kulon Progo</t>
+  </si>
+  <si>
+    <t>Kabupaten Bantul</t>
+  </si>
+  <si>
+    <t>Kabupaten Gunungkidul</t>
+  </si>
+  <si>
+    <t>Kabupaten Sleman</t>
+  </si>
+  <si>
+    <t>Kota Yogyakarta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,8 +1547,30 @@
       <color rgb="FF333333"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -994,6 +1580,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,7 +1617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1040,6 +1632,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2866,10 +3482,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2877,202 +3493,268 @@
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.5">
-      <c r="A2" s="4">
+    <row r="1" spans="1:3" ht="28.5">
+      <c r="A1" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="C2" s="4">
-        <v>16.07</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.5">
-      <c r="A3" s="4">
+      <c r="B1" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" s="9">
+        <v>73.03</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="C3" s="4">
-        <v>16.11</v>
+      <c r="B2" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" s="9">
+        <v>73.11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="9">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="9">
+        <v>73.08</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.5">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" s="4">
-        <v>16.04</v>
+      <c r="A4" s="9">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="C4" s="9">
+        <v>73.02</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.5">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="C5" s="4">
-        <v>16.03</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="42.75">
-      <c r="A6" s="4">
+      <c r="A5" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="C6" s="4">
-        <v>16.059999999999999</v>
+      <c r="B5" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="9">
+        <v>73.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="9">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="C6" s="9">
+        <v>73.06</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.5">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="C7" s="4">
-        <v>16.05</v>
+      <c r="A7" s="9">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" s="9">
+        <v>73.040000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.5">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C8" s="4">
-        <v>16.13</v>
+      <c r="A8" s="9">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="C8" s="9">
+        <v>73.010000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="C9" s="4">
-        <v>16.100000000000001</v>
+      <c r="A9" s="9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="C9" s="9">
+        <v>73.17</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.5">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="C10" s="4">
-        <v>16.02</v>
+      <c r="A10" s="9">
+        <v>10</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="C10" s="9">
+        <v>73.239999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.5">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C11" s="4">
-        <v>16.010000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="42.75">
-      <c r="A12" s="4">
+      <c r="A11" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="C12" s="4">
-        <v>16.09</v>
+      <c r="B11" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" s="9">
+        <v>73.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="9">
+        <v>12</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="9">
+        <v>73.09</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="42.75">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="C13" s="4">
-        <v>16.079999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.5">
-      <c r="A14" s="4">
+      <c r="A13" s="9">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="C14" s="4">
-        <v>16.12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4">
+      <c r="B13" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="C13" s="9">
+        <v>73.099999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="C15" s="4">
-        <v>16.73</v>
+      <c r="B14" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" s="9">
+        <v>73.150000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="42.75">
+      <c r="A15" s="9">
+        <v>15</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="C15" s="9">
+        <v>73.14</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="C16" s="4">
-        <v>16.72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4">
+      <c r="A16" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="C17" s="4">
-        <v>16.71</v>
+      <c r="B16" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="9">
+        <v>73.069999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.5">
+      <c r="A17" s="9">
+        <v>17</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="C17" s="9">
+        <v>73.12</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="C18" s="4">
-        <v>16.739999999999998</v>
+      <c r="A18" s="9">
+        <v>18</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="C18" s="9">
+        <v>73.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.5">
+      <c r="A19" s="9">
+        <v>19</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="C19" s="9">
+        <v>73.180000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.5">
+      <c r="A20" s="9">
+        <v>20</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C20" s="9">
+        <v>73.260000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="9">
+        <v>21</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="C21" s="9">
+        <v>73.13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="9">
+        <v>22</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="C22" s="9">
+        <v>73.709999999999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="9">
+        <v>23</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="C23" s="9">
+        <v>73.73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="9">
+        <v>24</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="C24" s="9">
+        <v>73.72</v>
       </c>
     </row>
   </sheetData>
@@ -3083,36 +3765,497 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" s="8">
+        <v>76.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="8">
+        <v>76.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="8">
+        <v>76.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="8">
+        <v>76.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" s="8">
+        <v>76.010000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" s="8">
+        <v>76.040000000000006</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.5">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="4">
+        <v>16.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="4">
+        <v>16.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="4">
+        <v>16.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="4">
+        <v>16.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="4">
+        <v>16.059999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C7" s="4">
+        <v>16.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="4">
+        <v>16.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" s="4">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.5">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C10" s="4">
+        <v>16.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" s="4">
+        <v>16.010000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="42.75">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C12" s="4">
+        <v>16.09</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="42.75">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C13" s="4">
+        <v>16.079999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.5">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C14" s="4">
+        <v>16.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.5">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="4">
+        <v>16.73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" s="4">
+        <v>16.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C17" s="4">
+        <v>16.71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C18" s="4">
+        <v>16.739999999999998</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>61.01</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>61.02</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9">
+        <v>61.03</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>61.04</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>61.05</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>61.06</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9">
+        <v>61.07</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>61.08</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9">
+        <v>61.09</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9">
+        <v>61.1</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9">
+        <v>61.11</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9">
+        <v>61.12</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9">
+        <v>61.71</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9">
+        <v>61.72</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>344</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3535,120 +4678,1623 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.5">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9">
+        <v>52.01</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9">
+        <v>52.02</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9">
+        <v>52.03</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>52.04</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>52.05</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>52.06</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9">
+        <v>52.07</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>52.08</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9">
+        <v>52.71</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9">
+        <v>52.72</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>63.01</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>63.02</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>63.03</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>63.04</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>63.05</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>63.06</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>63.07</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>63.08</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>63.09</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
+        <v>63.1</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>63.11</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12">
+        <v>63.71</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12">
+        <v>63.72</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>15.01</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>15.02</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>15.03</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>15.04</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>15.05</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>15.06</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>15.07</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>15.08</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>15.09</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
+        <v>15.71</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>15.72</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.5">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="12">
+        <v>71.010000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="C3" s="12">
+        <v>71.11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="C4" s="12">
+        <v>71.099999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="C5" s="12">
+        <v>71.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" s="12">
+        <v>71.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="C7" s="12">
+        <v>71.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="C8" s="12">
+        <v>71.040000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="C9" s="12">
+        <v>71.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.5">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="C10" s="12">
+        <v>71.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.5">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="C11" s="12">
+        <v>71.069999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="C12" s="12">
+        <v>71.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.5">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="C13" s="12">
+        <v>71.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="C14" s="12">
+        <v>71.739999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C15" s="12">
+        <v>71.709999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="C16" s="12">
+        <v>71.73</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>62.01</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>62.02</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>62.03</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>62.04</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>62.05</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>62.06</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>62.07</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>62.08</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>62.09</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
+        <v>62.1</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>62.11</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12">
+        <v>62.12</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12">
+        <v>62.13</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12">
+        <v>62.71</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>407</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>17.010000000000002</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>17.02</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>17.03</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>17.04</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>17.05</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>17.059999999999999</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>17.07</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>17.079999999999998</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>415</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>19.02</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>19.03</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>19.04</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>19.05</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>19.059999999999999</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>19.71</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>422</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="C2" s="12">
+        <v>92.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="C3" s="12">
+        <v>92.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4" s="12">
+        <v>92.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="C5" s="12">
+        <v>92.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="C6" s="12">
+        <v>92.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="C7" s="12">
+        <v>92.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="C8" s="12">
+        <v>92.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>430</v>
+      </c>
+      <c r="C9" s="12">
+        <v>92.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="C10" s="12">
+        <v>92.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="C11" s="12">
+        <v>92.09</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="C12" s="12">
+        <v>92.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="C13" s="12">
+        <v>92.07</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="C14" s="12">
+        <v>92.71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="C2" s="12">
+        <v>72.010000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.5">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C3" s="12">
+        <v>72.069999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>455</v>
+      </c>
+      <c r="C4" s="12">
+        <v>72.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="C5" s="12">
+        <v>72.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="C6" s="12">
+        <v>72.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>458</v>
+      </c>
+      <c r="C7" s="12">
+        <v>72.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="C8" s="12">
+        <v>72.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>460</v>
+      </c>
+      <c r="C9" s="12">
+        <v>72.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="C10" s="12">
+        <v>72.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="C11" s="12">
+        <v>72.09</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="C12" s="12">
+        <v>72.040000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="C13" s="12">
+        <v>72.099999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>465</v>
+      </c>
+      <c r="C14" s="12">
+        <v>72.709999999999994</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="C2" s="12">
+        <v>74.06</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="C3" s="12">
+        <v>74.040000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>438</v>
+      </c>
+      <c r="C4" s="12">
+        <v>74.150000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C5" s="12">
+        <v>74.14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6" s="12">
+        <v>74.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="C7" s="12">
+        <v>74.010000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="C8" s="12">
+        <v>74.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="C9" s="12">
+        <v>74.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="C10" s="12">
+        <v>74.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="C11" s="12">
+        <v>74.12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>446</v>
+      </c>
+      <c r="C12" s="12">
+        <v>74.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>447</v>
+      </c>
+      <c r="C13" s="12">
+        <v>74.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>448</v>
+      </c>
+      <c r="C14" s="12">
+        <v>74.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="C15" s="12">
+        <v>74.13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="C16" s="12">
+        <v>74.069999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>451</v>
+      </c>
+      <c r="C17" s="12">
+        <v>74.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>452</v>
+      </c>
+      <c r="C18" s="12">
+        <v>74.709999999999994</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4104,50 +6750,413 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>75.010000000000005</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>75.02</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>75.03</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>75.040000000000006</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>75.05</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>75.709999999999994</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>471</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" s="12">
+        <v>76.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" s="12">
+        <v>76.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="12">
+        <v>76.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="12">
+        <v>76.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" s="12">
+        <v>76.010000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" s="12">
+        <v>76.040000000000006</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>82.01</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>82.02</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>82.03</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>82.04</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>82.05</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>82.06</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>82.07</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>82.08</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>82.71</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
+        <v>82.72</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>481</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>34.01</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>34.020000000000003</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>34.03</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>34.04</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>34.71</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>